<commit_message>
update templates and examples
</commit_message>
<xml_diff>
--- a/Processes/Finance/Budgeting/General Department Budget Template.xlsx
+++ b/Processes/Finance/Budgeting/General Department Budget Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eichhornd\Desktop\Projekte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deich\git\Organization-Guide\Processes\Finance\Budgeting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD439AB9-5CD5-45C8-B18F-AB4C1D486AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A13091D-B986-4EBC-BB9F-03FD62566C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Costs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -233,9 +232,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Komma" xfId="1" builtinId="3"/>
-    <cellStyle name="Prozent" xfId="2" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -258,7 +257,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -295,7 +294,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -412,25 +411,25 @@
                 <c:formatCode>_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * "-"??_ ;_ @_ </c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2.5499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>2.42</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>3.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>2.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>2.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -496,7 +495,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1378944776"/>
@@ -527,6 +526,47 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:strRef>
+              <c:f>Costs!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>in TEUR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ " sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -555,7 +595,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1378947728"/>
@@ -603,7 +643,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -617,7 +657,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -654,7 +694,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -771,25 +811,25 @@
                 <c:formatCode>_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * "-"??_ ;_ @_ </c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5</c:v>
+                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5</c:v>
+                  <c:v>4.6499999999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5</c:v>
+                  <c:v>2.9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5</c:v>
+                  <c:v>3.3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -855,7 +895,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1378944776"/>
@@ -886,6 +926,47 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:strRef>
+              <c:f>Investments!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>in TEUR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ " sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -914,7 +995,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1378947728"/>
@@ -962,7 +1043,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2458,22 +2539,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L846"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="11.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="37.7265625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="1.54296875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="1.5703125" style="4" customWidth="1"/>
     <col min="4" max="10" width="9" style="9"/>
-    <col min="11" max="11" width="1.54296875" style="4" customWidth="1"/>
-    <col min="12" max="12" width="156.36328125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="1.5703125" style="4" customWidth="1"/>
+    <col min="12" max="12" width="156.42578125" style="9" customWidth="1"/>
     <col min="13" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="14.5" customHeight="1">
+    <row r="2" spans="2:12" ht="14.45" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
@@ -2577,25 +2656,25 @@
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="15">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="E6" s="15">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="F6" s="15">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="G6" s="15">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="H6" s="15">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="I6" s="15">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J6" s="15">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="K6" s="14"/>
       <c r="L6" s="16"/>
@@ -2606,25 +2685,25 @@
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="15">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="E7" s="15">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="F7" s="15">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="G7" s="15">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="H7" s="15">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="I7" s="15">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="J7" s="15">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K7" s="14"/>
       <c r="L7" s="16"/>
@@ -2644,7 +2723,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="15">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H8" s="15">
         <v>0</v>
@@ -2664,25 +2743,25 @@
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="15">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E9" s="15">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="F9" s="15">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="G9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" s="14"/>
       <c r="L9" s="16"/>
@@ -2696,22 +2775,22 @@
         <v>0</v>
       </c>
       <c r="E10" s="15">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F10" s="15">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G10" s="15">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="H10" s="15">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I10" s="15">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="J10" s="15">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="K10" s="14"/>
       <c r="L10" s="16"/>
@@ -2854,31 +2933,31 @@
       <c r="C22" s="6"/>
       <c r="D22" s="12">
         <f t="shared" ref="D22:I22" si="0">+SUM(D5:D21)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E22" s="12">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="F22" s="12">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2.42</v>
       </c>
       <c r="G22" s="12">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3.25</v>
       </c>
       <c r="H22" s="12">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2.75</v>
       </c>
       <c r="I22" s="12">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2.8</v>
       </c>
       <c r="J22" s="12">
         <f t="shared" ref="J22" si="1">+SUM(J5:J21)</f>
-        <v>1</v>
+        <v>2.85</v>
       </c>
       <c r="K22" s="6"/>
       <c r="L22" s="11"/>
@@ -4460,20 +4539,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:L846"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="11.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="2.54296875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="34.08984375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="1.54296875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="2.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="1.5703125" style="4" customWidth="1"/>
     <col min="4" max="10" width="9" style="9"/>
-    <col min="11" max="11" width="1.54296875" style="4" customWidth="1"/>
-    <col min="12" max="12" width="156.36328125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="1.5703125" style="4" customWidth="1"/>
+    <col min="12" max="12" width="156.42578125" style="9" customWidth="1"/>
     <col min="13" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="14.5" customHeight="1">
+    <row r="2" spans="2:12" ht="14.45" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
@@ -4577,25 +4656,25 @@
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="15">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E6" s="15">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="F6" s="15">
-        <v>0</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G6" s="15">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="H6" s="15">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="I6" s="15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J6" s="15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K6" s="14"/>
       <c r="L6" s="16"/>
@@ -4638,10 +4717,10 @@
         <v>0</v>
       </c>
       <c r="E8" s="15">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F8" s="15">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="G8" s="15">
         <v>0</v>
@@ -4650,7 +4729,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="15">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="J8" s="15">
         <v>0</v>
@@ -4812,32 +4891,32 @@
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="12">
-        <f>+SUM(D5:D21)</f>
-        <v>1.5</v>
+        <f t="shared" ref="D22:I22" si="0">+SUM(D5:D21)</f>
+        <v>3</v>
       </c>
       <c r="E22" s="12">
-        <f>+SUM(E5:E21)</f>
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>4.8</v>
       </c>
       <c r="F22" s="12">
-        <f>+SUM(F5:F21)</f>
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>4.6499999999999995</v>
       </c>
       <c r="G22" s="12">
-        <f>+SUM(G5:G21)</f>
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>2.9</v>
       </c>
       <c r="H22" s="12">
-        <f>+SUM(H5:H21)</f>
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>3.3</v>
       </c>
       <c r="I22" s="12">
-        <f>+SUM(I5:I21)</f>
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="J22" s="12">
-        <f t="shared" ref="J22" si="0">+SUM(J5:J21)</f>
-        <v>1.5</v>
+        <f t="shared" ref="J22" si="1">+SUM(J5:J21)</f>
+        <v>3.5</v>
       </c>
       <c r="K22" s="6"/>
       <c r="L22" s="11"/>

</xml_diff>